<commit_message>
Added labels to fund ratio upload,show and download (#988)
* Added labels to fund ratio upload,show and download

* Add label to fund ratios migration
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_ratios.xlsx
+++ b/public/sample_uploads/fund_ratios.xlsx
@@ -105,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t xml:space="preserve">Fund *</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t xml:space="preserve">End Date *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label</t>
   </si>
   <si>
     <t xml:space="preserve">Note</t>
@@ -307,36 +310,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,3248 +536,3267 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="O15" activeCellId="0" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="9.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="10" style="0" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="11" style="1" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="n">
         <v>23.45</v>
       </c>
-      <c r="G2" s="5" t="n">
+      <c r="G2" s="6" t="n">
         <v>44651</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="J2" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>1.4273</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>44651</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="J3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="n">
-        <v>1.4273</v>
-      </c>
-      <c r="G3" s="5" t="n">
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0.4367</v>
+      </c>
+      <c r="G4" s="6" t="n">
         <v>44651</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="H4" s="6"/>
+      <c r="J4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>1.8641</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>44651</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="J5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>27.95</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>44651</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="J6" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>0.4367</v>
-      </c>
-      <c r="G4" s="5" t="n">
+      <c r="F7" s="3" t="n">
+        <v>1.2773</v>
+      </c>
+      <c r="G7" s="7" t="n">
         <v>44651</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="H7" s="7"/>
+      <c r="J7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>1.8641</v>
-      </c>
-      <c r="G5" s="5" t="n">
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0.3367</v>
+      </c>
+      <c r="G8" s="7" t="n">
         <v>44651</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <v>27.95</v>
-      </c>
-      <c r="G6" s="6" t="n">
+      <c r="H8" s="7"/>
+      <c r="J8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>1.6141</v>
+      </c>
+      <c r="G9" s="7" t="n">
         <v>44651</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>1.2773</v>
-      </c>
-      <c r="G7" s="6" t="n">
+      <c r="H9" s="7"/>
+      <c r="J9" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0.4521</v>
+      </c>
+      <c r="G10" s="7" t="n">
         <v>44651</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>0.3367</v>
-      </c>
-      <c r="G8" s="6" t="n">
+      <c r="H10" s="7"/>
+      <c r="J10" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>1.4324</v>
+      </c>
+      <c r="G11" s="7" t="n">
         <v>44651</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>1.6141</v>
-      </c>
-      <c r="G9" s="6" t="n">
+      <c r="H11" s="7"/>
+      <c r="J11" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="7" t="n">
         <v>44651</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>0.4521</v>
-      </c>
-      <c r="G10" s="6" t="n">
+      <c r="H12" s="7"/>
+      <c r="J12" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>45.62</v>
+      </c>
+      <c r="G13" s="7" t="n">
         <v>44651</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>1.4324</v>
-      </c>
-      <c r="G11" s="6" t="n">
-        <v>44651</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G12" s="6" t="n">
-        <v>44651</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="4" t="n">
-        <v>45.62</v>
-      </c>
-      <c r="G13" s="6" t="n">
-        <v>44651</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>13</v>
+      <c r="H13" s="7"/>
+      <c r="J13" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I14" s="7"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I15" s="7"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I16" s="7"/>
+      <c r="J16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I17" s="7"/>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I18" s="7"/>
+      <c r="J18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I19" s="7"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I20" s="7"/>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I21" s="7"/>
+      <c r="J21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I22" s="7"/>
+      <c r="J22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I23" s="7"/>
+      <c r="J23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I24" s="7"/>
+      <c r="J24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I25" s="7"/>
+      <c r="J25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I26" s="7"/>
+      <c r="J26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I27" s="7"/>
+      <c r="J27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I28" s="7"/>
+      <c r="J28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I29" s="7"/>
+      <c r="J29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I30" s="7"/>
+      <c r="J30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I31" s="7"/>
+      <c r="J31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I32" s="7"/>
+      <c r="J32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I33" s="7"/>
+      <c r="J33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I34" s="7"/>
+      <c r="J34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I35" s="7"/>
+      <c r="J35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I36" s="7"/>
+      <c r="J36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I37" s="7"/>
+      <c r="J37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I38" s="7"/>
+      <c r="J38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I39" s="7"/>
+      <c r="J39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I40" s="7"/>
+      <c r="J40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I41" s="7"/>
+      <c r="J41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I42" s="7"/>
+      <c r="J42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I43" s="7"/>
+      <c r="J43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I44" s="7"/>
+      <c r="J44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I45" s="7"/>
+      <c r="J45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I46" s="7"/>
+      <c r="J46" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I47" s="7"/>
+      <c r="J47" s="8"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I48" s="7"/>
+      <c r="J48" s="8"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I49" s="7"/>
+      <c r="J49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I50" s="7"/>
+      <c r="J50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I51" s="7"/>
+      <c r="J51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I52" s="7"/>
+      <c r="J52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I53" s="7"/>
+      <c r="J53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I54" s="7"/>
+      <c r="J54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I55" s="7"/>
+      <c r="J55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I56" s="7"/>
+      <c r="J56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I57" s="7"/>
+      <c r="J57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I58" s="7"/>
+      <c r="J58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I59" s="7"/>
+      <c r="J59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I60" s="7"/>
+      <c r="J60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I61" s="7"/>
+      <c r="J61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I62" s="7"/>
+      <c r="J62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I63" s="7"/>
+      <c r="J63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I64" s="7"/>
+      <c r="J64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I65" s="7"/>
+      <c r="J65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I66" s="7"/>
+      <c r="J66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I67" s="7"/>
+      <c r="J67" s="8"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I68" s="7"/>
+      <c r="J68" s="8"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I69" s="7"/>
+      <c r="J69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I70" s="7"/>
+      <c r="J70" s="8"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I71" s="7"/>
+      <c r="J71" s="8"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I72" s="7"/>
+      <c r="J72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I73" s="7"/>
+      <c r="J73" s="8"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I74" s="7"/>
+      <c r="J74" s="8"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I75" s="7"/>
+      <c r="J75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I76" s="7"/>
+      <c r="J76" s="8"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I77" s="7"/>
+      <c r="J77" s="8"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I78" s="7"/>
+      <c r="J78" s="8"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I79" s="7"/>
+      <c r="J79" s="8"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I80" s="7"/>
+      <c r="J80" s="8"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I81" s="7"/>
+      <c r="J81" s="8"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I82" s="7"/>
+      <c r="J82" s="8"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I83" s="7"/>
+      <c r="J83" s="8"/>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I84" s="7"/>
+      <c r="J84" s="8"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I85" s="7"/>
+      <c r="J85" s="8"/>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I86" s="7"/>
+      <c r="J86" s="8"/>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I87" s="7"/>
+      <c r="J87" s="8"/>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I88" s="7"/>
+      <c r="J88" s="8"/>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I89" s="7"/>
+      <c r="J89" s="8"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I90" s="7"/>
+      <c r="J90" s="8"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I91" s="7"/>
+      <c r="J91" s="8"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I92" s="7"/>
+      <c r="J92" s="8"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I93" s="7"/>
+      <c r="J93" s="8"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I94" s="7"/>
+      <c r="J94" s="8"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I95" s="7"/>
+      <c r="J95" s="8"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I96" s="7"/>
+      <c r="J96" s="8"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I97" s="7"/>
+      <c r="J97" s="8"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I98" s="7"/>
+      <c r="J98" s="8"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I99" s="7"/>
+      <c r="J99" s="8"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I100" s="7"/>
+      <c r="J100" s="8"/>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I101" s="7"/>
+      <c r="J101" s="8"/>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I102" s="7"/>
+      <c r="J102" s="8"/>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I103" s="7"/>
+      <c r="J103" s="8"/>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I104" s="7"/>
+      <c r="J104" s="8"/>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I105" s="7"/>
+      <c r="J105" s="8"/>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I106" s="7"/>
+      <c r="J106" s="8"/>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I107" s="7"/>
+      <c r="J107" s="8"/>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I108" s="7"/>
+      <c r="J108" s="8"/>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I109" s="7"/>
+      <c r="J109" s="8"/>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I110" s="7"/>
+      <c r="J110" s="8"/>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I111" s="7"/>
+      <c r="J111" s="8"/>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I112" s="7"/>
+      <c r="J112" s="8"/>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I113" s="7"/>
+      <c r="J113" s="8"/>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I114" s="7"/>
+      <c r="J114" s="8"/>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I115" s="7"/>
+      <c r="J115" s="8"/>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I116" s="7"/>
+      <c r="J116" s="8"/>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I117" s="7"/>
+      <c r="J117" s="8"/>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I118" s="7"/>
+      <c r="J118" s="8"/>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I119" s="7"/>
+      <c r="J119" s="8"/>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I120" s="7"/>
+      <c r="J120" s="8"/>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I121" s="7"/>
+      <c r="J121" s="8"/>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I122" s="7"/>
+      <c r="J122" s="8"/>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I123" s="7"/>
+      <c r="J123" s="8"/>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I124" s="7"/>
+      <c r="J124" s="8"/>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I125" s="7"/>
+      <c r="J125" s="8"/>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I126" s="7"/>
+      <c r="J126" s="8"/>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I127" s="7"/>
+      <c r="J127" s="8"/>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I128" s="7"/>
+      <c r="J128" s="8"/>
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I129" s="7"/>
+      <c r="J129" s="8"/>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I130" s="7"/>
+      <c r="J130" s="8"/>
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I131" s="7"/>
+      <c r="J131" s="8"/>
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I132" s="7"/>
+      <c r="J132" s="8"/>
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I133" s="7"/>
+      <c r="J133" s="8"/>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I134" s="7"/>
+      <c r="J134" s="8"/>
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I135" s="7"/>
+      <c r="J135" s="8"/>
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I136" s="7"/>
+      <c r="J136" s="8"/>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I137" s="7"/>
+      <c r="J137" s="8"/>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I138" s="7"/>
+      <c r="J138" s="8"/>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I139" s="7"/>
+      <c r="J139" s="8"/>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I140" s="7"/>
+      <c r="J140" s="8"/>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I141" s="7"/>
+      <c r="J141" s="8"/>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I142" s="7"/>
+      <c r="J142" s="8"/>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I143" s="7"/>
+      <c r="J143" s="8"/>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I144" s="7"/>
+      <c r="J144" s="8"/>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I145" s="7"/>
+      <c r="J145" s="8"/>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I146" s="7"/>
+      <c r="J146" s="8"/>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I147" s="7"/>
+      <c r="J147" s="8"/>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I148" s="7"/>
+      <c r="J148" s="8"/>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I149" s="7"/>
+      <c r="J149" s="8"/>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I150" s="7"/>
+      <c r="J150" s="8"/>
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I151" s="7"/>
+      <c r="J151" s="8"/>
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I152" s="7"/>
+      <c r="J152" s="8"/>
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I153" s="7"/>
+      <c r="J153" s="8"/>
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I154" s="7"/>
+      <c r="J154" s="8"/>
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I155" s="7"/>
+      <c r="J155" s="8"/>
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I156" s="7"/>
+      <c r="J156" s="8"/>
     </row>
     <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I157" s="7"/>
+      <c r="J157" s="8"/>
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I158" s="7"/>
+      <c r="J158" s="8"/>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I159" s="7"/>
+      <c r="J159" s="8"/>
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I160" s="7"/>
+      <c r="J160" s="8"/>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I161" s="7"/>
+      <c r="J161" s="8"/>
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I162" s="7"/>
+      <c r="J162" s="8"/>
     </row>
     <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I163" s="7"/>
+      <c r="J163" s="8"/>
     </row>
     <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I164" s="7"/>
+      <c r="J164" s="8"/>
     </row>
     <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I165" s="7"/>
+      <c r="J165" s="8"/>
     </row>
     <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I166" s="7"/>
+      <c r="J166" s="8"/>
     </row>
     <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I167" s="7"/>
+      <c r="J167" s="8"/>
     </row>
     <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I168" s="7"/>
+      <c r="J168" s="8"/>
     </row>
     <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I169" s="7"/>
+      <c r="J169" s="8"/>
     </row>
     <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I170" s="7"/>
+      <c r="J170" s="8"/>
     </row>
     <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I171" s="7"/>
+      <c r="J171" s="8"/>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I172" s="7"/>
+      <c r="J172" s="8"/>
     </row>
     <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I173" s="7"/>
+      <c r="J173" s="8"/>
     </row>
     <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I174" s="7"/>
+      <c r="J174" s="8"/>
     </row>
     <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I175" s="7"/>
+      <c r="J175" s="8"/>
     </row>
     <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I176" s="7"/>
+      <c r="J176" s="8"/>
     </row>
     <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I177" s="7"/>
+      <c r="J177" s="8"/>
     </row>
     <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I178" s="7"/>
+      <c r="J178" s="8"/>
     </row>
     <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I179" s="7"/>
+      <c r="J179" s="8"/>
     </row>
     <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I180" s="7"/>
+      <c r="J180" s="8"/>
     </row>
     <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I181" s="7"/>
+      <c r="J181" s="8"/>
     </row>
     <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I182" s="7"/>
+      <c r="J182" s="8"/>
     </row>
     <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I183" s="7"/>
+      <c r="J183" s="8"/>
     </row>
     <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I184" s="7"/>
+      <c r="J184" s="8"/>
     </row>
     <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I185" s="7"/>
+      <c r="J185" s="8"/>
     </row>
     <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I186" s="7"/>
+      <c r="J186" s="8"/>
     </row>
     <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I187" s="7"/>
+      <c r="J187" s="8"/>
     </row>
     <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I188" s="7"/>
+      <c r="J188" s="8"/>
     </row>
     <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I189" s="7"/>
+      <c r="J189" s="8"/>
     </row>
     <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I190" s="7"/>
+      <c r="J190" s="8"/>
     </row>
     <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I191" s="7"/>
+      <c r="J191" s="8"/>
     </row>
     <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I192" s="7"/>
+      <c r="J192" s="8"/>
     </row>
     <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I193" s="7"/>
+      <c r="J193" s="8"/>
     </row>
     <row r="194" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I194" s="7"/>
+      <c r="J194" s="8"/>
     </row>
     <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I195" s="7"/>
+      <c r="J195" s="8"/>
     </row>
     <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I196" s="7"/>
+      <c r="J196" s="8"/>
     </row>
     <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I197" s="7"/>
+      <c r="J197" s="8"/>
     </row>
     <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I198" s="7"/>
+      <c r="J198" s="8"/>
     </row>
     <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I199" s="7"/>
+      <c r="J199" s="8"/>
     </row>
     <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I200" s="7"/>
+      <c r="J200" s="8"/>
     </row>
     <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I201" s="7"/>
+      <c r="J201" s="8"/>
     </row>
     <row r="202" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I202" s="7"/>
+      <c r="J202" s="8"/>
     </row>
     <row r="203" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I203" s="7"/>
+      <c r="J203" s="8"/>
     </row>
     <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I204" s="7"/>
+      <c r="J204" s="8"/>
     </row>
     <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I205" s="7"/>
+      <c r="J205" s="8"/>
     </row>
     <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I206" s="7"/>
+      <c r="J206" s="8"/>
     </row>
     <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I207" s="7"/>
+      <c r="J207" s="8"/>
     </row>
     <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I208" s="7"/>
+      <c r="J208" s="8"/>
     </row>
     <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I209" s="7"/>
+      <c r="J209" s="8"/>
     </row>
     <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I210" s="7"/>
+      <c r="J210" s="8"/>
     </row>
     <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I211" s="7"/>
+      <c r="J211" s="8"/>
     </row>
     <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I212" s="7"/>
+      <c r="J212" s="8"/>
     </row>
     <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I213" s="7"/>
+      <c r="J213" s="8"/>
     </row>
     <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I214" s="7"/>
+      <c r="J214" s="8"/>
     </row>
     <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I215" s="7"/>
+      <c r="J215" s="8"/>
     </row>
     <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I216" s="7"/>
+      <c r="J216" s="8"/>
     </row>
     <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I217" s="7"/>
+      <c r="J217" s="8"/>
     </row>
     <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I218" s="7"/>
+      <c r="J218" s="8"/>
     </row>
     <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I219" s="7"/>
+      <c r="J219" s="8"/>
     </row>
     <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I220" s="7"/>
+      <c r="J220" s="8"/>
     </row>
     <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I221" s="7"/>
+      <c r="J221" s="8"/>
     </row>
     <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I222" s="7"/>
+      <c r="J222" s="8"/>
     </row>
     <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I223" s="7"/>
+      <c r="J223" s="8"/>
     </row>
     <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I224" s="7"/>
+      <c r="J224" s="8"/>
     </row>
     <row r="225" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I225" s="7"/>
+      <c r="J225" s="8"/>
     </row>
     <row r="226" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I226" s="7"/>
+      <c r="J226" s="8"/>
     </row>
     <row r="227" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I227" s="7"/>
+      <c r="J227" s="8"/>
     </row>
     <row r="228" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I228" s="7"/>
+      <c r="J228" s="8"/>
     </row>
     <row r="229" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I229" s="7"/>
+      <c r="J229" s="8"/>
     </row>
     <row r="230" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I230" s="7"/>
+      <c r="J230" s="8"/>
     </row>
     <row r="231" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I231" s="7"/>
+      <c r="J231" s="8"/>
     </row>
     <row r="232" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I232" s="7"/>
+      <c r="J232" s="8"/>
     </row>
     <row r="233" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I233" s="7"/>
+      <c r="J233" s="8"/>
     </row>
     <row r="234" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I234" s="7"/>
+      <c r="J234" s="8"/>
     </row>
     <row r="235" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I235" s="7"/>
+      <c r="J235" s="8"/>
     </row>
     <row r="236" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I236" s="7"/>
+      <c r="J236" s="8"/>
     </row>
     <row r="237" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I237" s="7"/>
+      <c r="J237" s="8"/>
     </row>
     <row r="238" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I238" s="7"/>
+      <c r="J238" s="8"/>
     </row>
     <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I239" s="7"/>
+      <c r="J239" s="8"/>
     </row>
     <row r="240" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I240" s="7"/>
+      <c r="J240" s="8"/>
     </row>
     <row r="241" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I241" s="7"/>
+      <c r="J241" s="8"/>
     </row>
     <row r="242" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I242" s="7"/>
+      <c r="J242" s="8"/>
     </row>
     <row r="243" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I243" s="7"/>
+      <c r="J243" s="8"/>
     </row>
     <row r="244" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I244" s="7"/>
+      <c r="J244" s="8"/>
     </row>
     <row r="245" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I245" s="7"/>
+      <c r="J245" s="8"/>
     </row>
     <row r="246" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I246" s="7"/>
+      <c r="J246" s="8"/>
     </row>
     <row r="247" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I247" s="7"/>
+      <c r="J247" s="8"/>
     </row>
     <row r="248" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I248" s="7"/>
+      <c r="J248" s="8"/>
     </row>
     <row r="249" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I249" s="7"/>
+      <c r="J249" s="8"/>
     </row>
     <row r="250" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I250" s="7"/>
+      <c r="J250" s="8"/>
     </row>
     <row r="251" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I251" s="7"/>
+      <c r="J251" s="8"/>
     </row>
     <row r="252" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I252" s="7"/>
+      <c r="J252" s="8"/>
     </row>
     <row r="253" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I253" s="7"/>
+      <c r="J253" s="8"/>
     </row>
     <row r="254" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I254" s="7"/>
+      <c r="J254" s="8"/>
     </row>
     <row r="255" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I255" s="7"/>
+      <c r="J255" s="8"/>
     </row>
     <row r="256" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I256" s="7"/>
+      <c r="J256" s="8"/>
     </row>
     <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I257" s="7"/>
+      <c r="J257" s="8"/>
     </row>
     <row r="258" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I258" s="7"/>
+      <c r="J258" s="8"/>
     </row>
     <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I259" s="7"/>
+      <c r="J259" s="8"/>
     </row>
     <row r="260" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I260" s="7"/>
+      <c r="J260" s="8"/>
     </row>
     <row r="261" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I261" s="7"/>
+      <c r="J261" s="8"/>
     </row>
     <row r="262" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I262" s="7"/>
+      <c r="J262" s="8"/>
     </row>
     <row r="263" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I263" s="7"/>
+      <c r="J263" s="8"/>
     </row>
     <row r="264" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I264" s="7"/>
+      <c r="J264" s="8"/>
     </row>
     <row r="265" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I265" s="7"/>
+      <c r="J265" s="8"/>
     </row>
     <row r="266" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I266" s="7"/>
+      <c r="J266" s="8"/>
     </row>
     <row r="267" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I267" s="7"/>
+      <c r="J267" s="8"/>
     </row>
     <row r="268" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I268" s="7"/>
+      <c r="J268" s="8"/>
     </row>
     <row r="269" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I269" s="7"/>
+      <c r="J269" s="8"/>
     </row>
     <row r="270" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I270" s="7"/>
+      <c r="J270" s="8"/>
     </row>
     <row r="271" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I271" s="7"/>
+      <c r="J271" s="8"/>
     </row>
     <row r="272" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I272" s="7"/>
+      <c r="J272" s="8"/>
     </row>
     <row r="273" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I273" s="7"/>
+      <c r="J273" s="8"/>
     </row>
     <row r="274" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I274" s="7"/>
+      <c r="J274" s="8"/>
     </row>
     <row r="275" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I275" s="7"/>
+      <c r="J275" s="8"/>
     </row>
     <row r="276" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I276" s="7"/>
+      <c r="J276" s="8"/>
     </row>
     <row r="277" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I277" s="7"/>
+      <c r="J277" s="8"/>
     </row>
     <row r="278" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I278" s="7"/>
+      <c r="J278" s="8"/>
     </row>
     <row r="279" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I279" s="7"/>
+      <c r="J279" s="8"/>
     </row>
     <row r="280" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I280" s="7"/>
+      <c r="J280" s="8"/>
     </row>
     <row r="281" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I281" s="7"/>
+      <c r="J281" s="8"/>
     </row>
     <row r="282" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I282" s="7"/>
+      <c r="J282" s="8"/>
     </row>
     <row r="283" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I283" s="7"/>
+      <c r="J283" s="8"/>
     </row>
     <row r="284" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I284" s="7"/>
+      <c r="J284" s="8"/>
     </row>
     <row r="285" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I285" s="7"/>
+      <c r="J285" s="8"/>
     </row>
     <row r="286" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I286" s="7"/>
+      <c r="J286" s="8"/>
     </row>
     <row r="287" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I287" s="7"/>
+      <c r="J287" s="8"/>
     </row>
     <row r="288" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I288" s="7"/>
+      <c r="J288" s="8"/>
     </row>
     <row r="289" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I289" s="7"/>
+      <c r="J289" s="8"/>
     </row>
     <row r="290" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I290" s="7"/>
+      <c r="J290" s="8"/>
     </row>
     <row r="291" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I291" s="7"/>
+      <c r="J291" s="8"/>
     </row>
     <row r="292" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I292" s="7"/>
+      <c r="J292" s="8"/>
     </row>
     <row r="293" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I293" s="7"/>
+      <c r="J293" s="8"/>
     </row>
     <row r="294" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I294" s="7"/>
+      <c r="J294" s="8"/>
     </row>
     <row r="295" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I295" s="7"/>
+      <c r="J295" s="8"/>
     </row>
     <row r="296" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I296" s="7"/>
+      <c r="J296" s="8"/>
     </row>
     <row r="297" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I297" s="7"/>
+      <c r="J297" s="8"/>
     </row>
     <row r="298" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I298" s="7"/>
+      <c r="J298" s="8"/>
     </row>
     <row r="299" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I299" s="7"/>
+      <c r="J299" s="8"/>
     </row>
     <row r="300" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I300" s="7"/>
+      <c r="J300" s="8"/>
     </row>
     <row r="301" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I301" s="7"/>
+      <c r="J301" s="8"/>
     </row>
     <row r="302" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I302" s="7"/>
+      <c r="J302" s="8"/>
     </row>
     <row r="303" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I303" s="7"/>
+      <c r="J303" s="8"/>
     </row>
     <row r="304" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I304" s="7"/>
+      <c r="J304" s="8"/>
     </row>
     <row r="305" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I305" s="7"/>
+      <c r="J305" s="8"/>
     </row>
     <row r="306" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I306" s="7"/>
+      <c r="J306" s="8"/>
     </row>
     <row r="307" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I307" s="7"/>
+      <c r="J307" s="8"/>
     </row>
     <row r="308" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I308" s="7"/>
+      <c r="J308" s="8"/>
     </row>
     <row r="309" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I309" s="7"/>
+      <c r="J309" s="8"/>
     </row>
     <row r="310" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I310" s="7"/>
+      <c r="J310" s="8"/>
     </row>
     <row r="311" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I311" s="7"/>
+      <c r="J311" s="8"/>
     </row>
     <row r="312" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I312" s="7"/>
+      <c r="J312" s="8"/>
     </row>
     <row r="313" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I313" s="7"/>
+      <c r="J313" s="8"/>
     </row>
     <row r="314" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I314" s="7"/>
+      <c r="J314" s="8"/>
     </row>
     <row r="315" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I315" s="7"/>
+      <c r="J315" s="8"/>
     </row>
     <row r="316" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I316" s="7"/>
+      <c r="J316" s="8"/>
     </row>
     <row r="317" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I317" s="7"/>
+      <c r="J317" s="8"/>
     </row>
     <row r="318" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I318" s="7"/>
+      <c r="J318" s="8"/>
     </row>
     <row r="319" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I319" s="7"/>
+      <c r="J319" s="8"/>
     </row>
     <row r="320" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I320" s="7"/>
+      <c r="J320" s="8"/>
     </row>
     <row r="321" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I321" s="7"/>
+      <c r="J321" s="8"/>
     </row>
     <row r="322" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I322" s="7"/>
+      <c r="J322" s="8"/>
     </row>
     <row r="323" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I323" s="7"/>
+      <c r="J323" s="8"/>
     </row>
     <row r="324" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I324" s="7"/>
+      <c r="J324" s="8"/>
     </row>
     <row r="325" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I325" s="7"/>
+      <c r="J325" s="8"/>
     </row>
     <row r="326" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I326" s="7"/>
+      <c r="J326" s="8"/>
     </row>
     <row r="327" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I327" s="7"/>
+      <c r="J327" s="8"/>
     </row>
     <row r="328" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I328" s="7"/>
+      <c r="J328" s="8"/>
     </row>
     <row r="329" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I329" s="7"/>
+      <c r="J329" s="8"/>
     </row>
     <row r="330" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I330" s="7"/>
+      <c r="J330" s="8"/>
     </row>
     <row r="331" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I331" s="7"/>
+      <c r="J331" s="8"/>
     </row>
     <row r="332" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I332" s="7"/>
+      <c r="J332" s="8"/>
     </row>
     <row r="333" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I333" s="7"/>
+      <c r="J333" s="8"/>
     </row>
     <row r="334" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I334" s="7"/>
+      <c r="J334" s="8"/>
     </row>
     <row r="335" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I335" s="7"/>
+      <c r="J335" s="8"/>
     </row>
     <row r="336" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I336" s="7"/>
+      <c r="J336" s="8"/>
     </row>
     <row r="337" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I337" s="7"/>
+      <c r="J337" s="8"/>
     </row>
     <row r="338" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I338" s="7"/>
+      <c r="J338" s="8"/>
     </row>
     <row r="339" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I339" s="7"/>
+      <c r="J339" s="8"/>
     </row>
     <row r="340" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I340" s="7"/>
+      <c r="J340" s="8"/>
     </row>
     <row r="341" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I341" s="7"/>
+      <c r="J341" s="8"/>
     </row>
     <row r="342" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I342" s="7"/>
+      <c r="J342" s="8"/>
     </row>
     <row r="343" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I343" s="7"/>
+      <c r="J343" s="8"/>
     </row>
     <row r="344" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I344" s="7"/>
+      <c r="J344" s="8"/>
     </row>
     <row r="345" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I345" s="7"/>
+      <c r="J345" s="8"/>
     </row>
     <row r="346" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I346" s="7"/>
+      <c r="J346" s="8"/>
     </row>
     <row r="347" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I347" s="7"/>
+      <c r="J347" s="8"/>
     </row>
     <row r="348" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I348" s="7"/>
+      <c r="J348" s="8"/>
     </row>
     <row r="349" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I349" s="7"/>
+      <c r="J349" s="8"/>
     </row>
     <row r="350" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I350" s="7"/>
+      <c r="J350" s="8"/>
     </row>
     <row r="351" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I351" s="7"/>
+      <c r="J351" s="8"/>
     </row>
     <row r="352" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I352" s="7"/>
+      <c r="J352" s="8"/>
     </row>
     <row r="353" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I353" s="7"/>
+      <c r="J353" s="8"/>
     </row>
     <row r="354" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I354" s="7"/>
+      <c r="J354" s="8"/>
     </row>
     <row r="355" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I355" s="7"/>
+      <c r="J355" s="8"/>
     </row>
     <row r="356" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I356" s="7"/>
+      <c r="J356" s="8"/>
     </row>
     <row r="357" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I357" s="7"/>
+      <c r="J357" s="8"/>
     </row>
     <row r="358" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I358" s="7"/>
+      <c r="J358" s="8"/>
     </row>
     <row r="359" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I359" s="7"/>
+      <c r="J359" s="8"/>
     </row>
     <row r="360" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I360" s="7"/>
+      <c r="J360" s="8"/>
     </row>
     <row r="361" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I361" s="7"/>
+      <c r="J361" s="8"/>
     </row>
     <row r="362" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I362" s="7"/>
+      <c r="J362" s="8"/>
     </row>
     <row r="363" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I363" s="7"/>
+      <c r="J363" s="8"/>
     </row>
     <row r="364" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I364" s="7"/>
+      <c r="J364" s="8"/>
     </row>
     <row r="365" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I365" s="7"/>
+      <c r="J365" s="8"/>
     </row>
     <row r="366" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I366" s="7"/>
+      <c r="J366" s="8"/>
     </row>
     <row r="367" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I367" s="7"/>
+      <c r="J367" s="8"/>
     </row>
     <row r="368" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I368" s="7"/>
+      <c r="J368" s="8"/>
     </row>
     <row r="369" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I369" s="7"/>
+      <c r="J369" s="8"/>
     </row>
     <row r="370" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I370" s="7"/>
+      <c r="J370" s="8"/>
     </row>
     <row r="371" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I371" s="7"/>
+      <c r="J371" s="8"/>
     </row>
     <row r="372" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I372" s="7"/>
+      <c r="J372" s="8"/>
     </row>
     <row r="373" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I373" s="7"/>
+      <c r="J373" s="8"/>
     </row>
     <row r="374" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I374" s="7"/>
+      <c r="J374" s="8"/>
     </row>
     <row r="375" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I375" s="7"/>
+      <c r="J375" s="8"/>
     </row>
     <row r="376" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I376" s="7"/>
+      <c r="J376" s="8"/>
     </row>
     <row r="377" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I377" s="7"/>
+      <c r="J377" s="8"/>
     </row>
     <row r="378" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I378" s="7"/>
+      <c r="J378" s="8"/>
     </row>
     <row r="379" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I379" s="7"/>
+      <c r="J379" s="8"/>
     </row>
     <row r="380" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I380" s="7"/>
+      <c r="J380" s="8"/>
     </row>
     <row r="381" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I381" s="7"/>
+      <c r="J381" s="8"/>
     </row>
     <row r="382" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I382" s="7"/>
+      <c r="J382" s="8"/>
     </row>
     <row r="383" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I383" s="7"/>
+      <c r="J383" s="8"/>
     </row>
     <row r="384" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I384" s="7"/>
+      <c r="J384" s="8"/>
     </row>
     <row r="385" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I385" s="7"/>
+      <c r="J385" s="8"/>
     </row>
     <row r="386" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I386" s="7"/>
+      <c r="J386" s="8"/>
     </row>
     <row r="387" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I387" s="7"/>
+      <c r="J387" s="8"/>
     </row>
     <row r="388" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I388" s="7"/>
+      <c r="J388" s="8"/>
     </row>
     <row r="389" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I389" s="7"/>
+      <c r="J389" s="8"/>
     </row>
     <row r="390" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I390" s="7"/>
+      <c r="J390" s="8"/>
     </row>
     <row r="391" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I391" s="7"/>
+      <c r="J391" s="8"/>
     </row>
     <row r="392" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I392" s="7"/>
+      <c r="J392" s="8"/>
     </row>
     <row r="393" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I393" s="7"/>
+      <c r="J393" s="8"/>
     </row>
     <row r="394" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I394" s="7"/>
+      <c r="J394" s="8"/>
     </row>
     <row r="395" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I395" s="7"/>
+      <c r="J395" s="8"/>
     </row>
     <row r="396" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I396" s="7"/>
+      <c r="J396" s="8"/>
     </row>
     <row r="397" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I397" s="7"/>
+      <c r="J397" s="8"/>
     </row>
     <row r="398" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I398" s="7"/>
+      <c r="J398" s="8"/>
     </row>
     <row r="399" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I399" s="7"/>
+      <c r="J399" s="8"/>
     </row>
     <row r="400" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I400" s="7"/>
+      <c r="J400" s="8"/>
     </row>
     <row r="401" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I401" s="7"/>
+      <c r="J401" s="8"/>
     </row>
     <row r="402" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I402" s="7"/>
+      <c r="J402" s="8"/>
     </row>
     <row r="403" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I403" s="7"/>
+      <c r="J403" s="8"/>
     </row>
     <row r="404" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I404" s="7"/>
+      <c r="J404" s="8"/>
     </row>
     <row r="405" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I405" s="7"/>
+      <c r="J405" s="8"/>
     </row>
     <row r="406" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I406" s="7"/>
+      <c r="J406" s="8"/>
     </row>
     <row r="407" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I407" s="7"/>
+      <c r="J407" s="8"/>
     </row>
     <row r="408" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I408" s="7"/>
+      <c r="J408" s="8"/>
     </row>
     <row r="409" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I409" s="7"/>
+      <c r="J409" s="8"/>
     </row>
     <row r="410" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I410" s="7"/>
+      <c r="J410" s="8"/>
     </row>
     <row r="411" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I411" s="7"/>
+      <c r="J411" s="8"/>
     </row>
     <row r="412" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I412" s="7"/>
+      <c r="J412" s="8"/>
     </row>
     <row r="413" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I413" s="7"/>
+      <c r="J413" s="8"/>
     </row>
     <row r="414" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I414" s="7"/>
+      <c r="J414" s="8"/>
     </row>
     <row r="415" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I415" s="7"/>
+      <c r="J415" s="8"/>
     </row>
     <row r="416" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I416" s="7"/>
+      <c r="J416" s="8"/>
     </row>
     <row r="417" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I417" s="7"/>
+      <c r="J417" s="8"/>
     </row>
     <row r="418" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I418" s="7"/>
+      <c r="J418" s="8"/>
     </row>
     <row r="419" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I419" s="7"/>
+      <c r="J419" s="8"/>
     </row>
     <row r="420" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I420" s="7"/>
+      <c r="J420" s="8"/>
     </row>
     <row r="421" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I421" s="7"/>
+      <c r="J421" s="8"/>
     </row>
     <row r="422" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I422" s="7"/>
+      <c r="J422" s="8"/>
     </row>
     <row r="423" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I423" s="7"/>
+      <c r="J423" s="8"/>
     </row>
     <row r="424" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I424" s="7"/>
+      <c r="J424" s="8"/>
     </row>
     <row r="425" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I425" s="7"/>
+      <c r="J425" s="8"/>
     </row>
     <row r="426" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I426" s="7"/>
+      <c r="J426" s="8"/>
     </row>
     <row r="427" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I427" s="7"/>
+      <c r="J427" s="8"/>
     </row>
     <row r="428" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I428" s="7"/>
+      <c r="J428" s="8"/>
     </row>
     <row r="429" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I429" s="7"/>
+      <c r="J429" s="8"/>
     </row>
     <row r="430" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I430" s="7"/>
+      <c r="J430" s="8"/>
     </row>
     <row r="431" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I431" s="7"/>
+      <c r="J431" s="8"/>
     </row>
     <row r="432" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I432" s="7"/>
+      <c r="J432" s="8"/>
     </row>
     <row r="433" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I433" s="7"/>
+      <c r="J433" s="8"/>
     </row>
     <row r="434" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I434" s="7"/>
+      <c r="J434" s="8"/>
     </row>
     <row r="435" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I435" s="7"/>
+      <c r="J435" s="8"/>
     </row>
     <row r="436" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I436" s="7"/>
+      <c r="J436" s="8"/>
     </row>
     <row r="437" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I437" s="7"/>
+      <c r="J437" s="8"/>
     </row>
     <row r="438" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I438" s="7"/>
+      <c r="J438" s="8"/>
     </row>
     <row r="439" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I439" s="7"/>
+      <c r="J439" s="8"/>
     </row>
     <row r="440" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I440" s="7"/>
+      <c r="J440" s="8"/>
     </row>
     <row r="441" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I441" s="7"/>
+      <c r="J441" s="8"/>
     </row>
     <row r="442" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I442" s="7"/>
+      <c r="J442" s="8"/>
     </row>
     <row r="443" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I443" s="7"/>
+      <c r="J443" s="8"/>
     </row>
     <row r="444" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I444" s="7"/>
+      <c r="J444" s="8"/>
     </row>
     <row r="445" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I445" s="7"/>
+      <c r="J445" s="8"/>
     </row>
     <row r="446" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I446" s="7"/>
+      <c r="J446" s="8"/>
     </row>
     <row r="447" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I447" s="7"/>
+      <c r="J447" s="8"/>
     </row>
     <row r="448" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I448" s="7"/>
+      <c r="J448" s="8"/>
     </row>
     <row r="449" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I449" s="7"/>
+      <c r="J449" s="8"/>
     </row>
     <row r="450" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I450" s="7"/>
+      <c r="J450" s="8"/>
     </row>
     <row r="451" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I451" s="7"/>
+      <c r="J451" s="8"/>
     </row>
     <row r="452" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I452" s="7"/>
+      <c r="J452" s="8"/>
     </row>
     <row r="453" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I453" s="7"/>
+      <c r="J453" s="8"/>
     </row>
     <row r="454" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I454" s="7"/>
+      <c r="J454" s="8"/>
     </row>
     <row r="455" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I455" s="7"/>
+      <c r="J455" s="8"/>
     </row>
     <row r="456" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I456" s="7"/>
+      <c r="J456" s="8"/>
     </row>
     <row r="457" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I457" s="7"/>
+      <c r="J457" s="8"/>
     </row>
     <row r="458" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I458" s="7"/>
+      <c r="J458" s="8"/>
     </row>
     <row r="459" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I459" s="7"/>
+      <c r="J459" s="8"/>
     </row>
     <row r="460" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I460" s="7"/>
+      <c r="J460" s="8"/>
     </row>
     <row r="461" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I461" s="7"/>
+      <c r="J461" s="8"/>
     </row>
     <row r="462" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I462" s="7"/>
+      <c r="J462" s="8"/>
     </row>
     <row r="463" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I463" s="7"/>
+      <c r="J463" s="8"/>
     </row>
     <row r="464" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I464" s="7"/>
+      <c r="J464" s="8"/>
     </row>
     <row r="465" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I465" s="7"/>
+      <c r="J465" s="8"/>
     </row>
     <row r="466" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I466" s="7"/>
+      <c r="J466" s="8"/>
     </row>
     <row r="467" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I467" s="7"/>
+      <c r="J467" s="8"/>
     </row>
     <row r="468" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I468" s="7"/>
+      <c r="J468" s="8"/>
     </row>
     <row r="469" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I469" s="7"/>
+      <c r="J469" s="8"/>
     </row>
     <row r="470" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I470" s="7"/>
+      <c r="J470" s="8"/>
     </row>
     <row r="471" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I471" s="7"/>
+      <c r="J471" s="8"/>
     </row>
     <row r="472" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I472" s="7"/>
+      <c r="J472" s="8"/>
     </row>
     <row r="473" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I473" s="7"/>
+      <c r="J473" s="8"/>
     </row>
     <row r="474" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I474" s="7"/>
+      <c r="J474" s="8"/>
     </row>
     <row r="475" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I475" s="7"/>
+      <c r="J475" s="8"/>
     </row>
     <row r="476" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I476" s="7"/>
+      <c r="J476" s="8"/>
     </row>
     <row r="477" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I477" s="7"/>
+      <c r="J477" s="8"/>
     </row>
     <row r="478" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I478" s="7"/>
+      <c r="J478" s="8"/>
     </row>
     <row r="479" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I479" s="7"/>
+      <c r="J479" s="8"/>
     </row>
     <row r="480" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I480" s="7"/>
+      <c r="J480" s="8"/>
     </row>
     <row r="481" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I481" s="7"/>
+      <c r="J481" s="8"/>
     </row>
     <row r="482" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I482" s="7"/>
+      <c r="J482" s="8"/>
     </row>
     <row r="483" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I483" s="7"/>
+      <c r="J483" s="8"/>
     </row>
     <row r="484" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I484" s="7"/>
+      <c r="J484" s="8"/>
     </row>
     <row r="485" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I485" s="7"/>
+      <c r="J485" s="8"/>
     </row>
     <row r="486" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I486" s="7"/>
+      <c r="J486" s="8"/>
     </row>
     <row r="487" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I487" s="7"/>
+      <c r="J487" s="8"/>
     </row>
     <row r="488" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I488" s="7"/>
+      <c r="J488" s="8"/>
     </row>
     <row r="489" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I489" s="7"/>
+      <c r="J489" s="8"/>
     </row>
     <row r="490" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I490" s="7"/>
+      <c r="J490" s="8"/>
     </row>
     <row r="491" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I491" s="7"/>
+      <c r="J491" s="8"/>
     </row>
     <row r="492" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I492" s="7"/>
+      <c r="J492" s="8"/>
     </row>
     <row r="493" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I493" s="7"/>
+      <c r="J493" s="8"/>
     </row>
     <row r="494" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I494" s="7"/>
+      <c r="J494" s="8"/>
     </row>
     <row r="495" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I495" s="7"/>
+      <c r="J495" s="8"/>
     </row>
     <row r="496" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I496" s="7"/>
+      <c r="J496" s="8"/>
     </row>
     <row r="497" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I497" s="7"/>
+      <c r="J497" s="8"/>
     </row>
     <row r="498" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I498" s="7"/>
+      <c r="J498" s="8"/>
     </row>
     <row r="499" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I499" s="7"/>
+      <c r="J499" s="8"/>
     </row>
     <row r="500" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I500" s="7"/>
+      <c r="J500" s="8"/>
     </row>
     <row r="501" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I501" s="7"/>
+      <c r="J501" s="8"/>
     </row>
     <row r="502" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I502" s="7"/>
+      <c r="J502" s="8"/>
     </row>
     <row r="503" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I503" s="7"/>
+      <c r="J503" s="8"/>
     </row>
     <row r="504" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I504" s="7"/>
+      <c r="J504" s="8"/>
     </row>
     <row r="505" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I505" s="7"/>
+      <c r="J505" s="8"/>
     </row>
     <row r="506" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I506" s="7"/>
+      <c r="J506" s="8"/>
     </row>
     <row r="507" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I507" s="7"/>
+      <c r="J507" s="8"/>
     </row>
     <row r="508" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I508" s="7"/>
+      <c r="J508" s="8"/>
     </row>
     <row r="509" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I509" s="7"/>
+      <c r="J509" s="8"/>
     </row>
     <row r="510" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I510" s="7"/>
+      <c r="J510" s="8"/>
     </row>
     <row r="511" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I511" s="7"/>
+      <c r="J511" s="8"/>
     </row>
     <row r="512" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I512" s="7"/>
+      <c r="J512" s="8"/>
     </row>
     <row r="513" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I513" s="7"/>
+      <c r="J513" s="8"/>
     </row>
     <row r="514" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I514" s="7"/>
+      <c r="J514" s="8"/>
     </row>
     <row r="515" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I515" s="7"/>
+      <c r="J515" s="8"/>
     </row>
     <row r="516" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I516" s="7"/>
+      <c r="J516" s="8"/>
     </row>
     <row r="517" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I517" s="7"/>
+      <c r="J517" s="8"/>
     </row>
     <row r="518" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I518" s="7"/>
+      <c r="J518" s="8"/>
     </row>
     <row r="519" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I519" s="7"/>
+      <c r="J519" s="8"/>
     </row>
     <row r="520" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I520" s="7"/>
+      <c r="J520" s="8"/>
     </row>
     <row r="521" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I521" s="7"/>
+      <c r="J521" s="8"/>
     </row>
     <row r="522" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I522" s="7"/>
+      <c r="J522" s="8"/>
     </row>
     <row r="523" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I523" s="7"/>
+      <c r="J523" s="8"/>
     </row>
     <row r="524" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I524" s="7"/>
+      <c r="J524" s="8"/>
     </row>
     <row r="525" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I525" s="7"/>
+      <c r="J525" s="8"/>
     </row>
     <row r="526" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I526" s="7"/>
+      <c r="J526" s="8"/>
     </row>
     <row r="527" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I527" s="7"/>
+      <c r="J527" s="8"/>
     </row>
     <row r="528" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I528" s="7"/>
+      <c r="J528" s="8"/>
     </row>
     <row r="529" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I529" s="7"/>
+      <c r="J529" s="8"/>
     </row>
     <row r="530" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I530" s="7"/>
+      <c r="J530" s="8"/>
     </row>
     <row r="531" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I531" s="7"/>
+      <c r="J531" s="8"/>
     </row>
     <row r="532" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I532" s="7"/>
+      <c r="J532" s="8"/>
     </row>
     <row r="533" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I533" s="7"/>
+      <c r="J533" s="8"/>
     </row>
     <row r="534" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I534" s="7"/>
+      <c r="J534" s="8"/>
     </row>
     <row r="535" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I535" s="7"/>
+      <c r="J535" s="8"/>
     </row>
     <row r="536" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I536" s="7"/>
+      <c r="J536" s="8"/>
     </row>
     <row r="537" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I537" s="7"/>
+      <c r="J537" s="8"/>
     </row>
     <row r="538" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I538" s="7"/>
+      <c r="J538" s="8"/>
     </row>
     <row r="539" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I539" s="7"/>
+      <c r="J539" s="8"/>
     </row>
     <row r="540" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I540" s="7"/>
+      <c r="J540" s="8"/>
     </row>
     <row r="541" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I541" s="7"/>
+      <c r="J541" s="8"/>
     </row>
     <row r="542" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I542" s="7"/>
+      <c r="J542" s="8"/>
     </row>
     <row r="543" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I543" s="7"/>
+      <c r="J543" s="8"/>
     </row>
     <row r="544" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I544" s="7"/>
+      <c r="J544" s="8"/>
     </row>
     <row r="545" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I545" s="7"/>
+      <c r="J545" s="8"/>
     </row>
     <row r="546" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I546" s="7"/>
+      <c r="J546" s="8"/>
     </row>
     <row r="547" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I547" s="7"/>
+      <c r="J547" s="8"/>
     </row>
     <row r="548" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I548" s="7"/>
+      <c r="J548" s="8"/>
     </row>
     <row r="549" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I549" s="7"/>
+      <c r="J549" s="8"/>
     </row>
     <row r="550" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I550" s="7"/>
+      <c r="J550" s="8"/>
     </row>
     <row r="551" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I551" s="7"/>
+      <c r="J551" s="8"/>
     </row>
     <row r="552" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I552" s="7"/>
+      <c r="J552" s="8"/>
     </row>
     <row r="553" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I553" s="7"/>
+      <c r="J553" s="8"/>
     </row>
     <row r="554" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I554" s="7"/>
+      <c r="J554" s="8"/>
     </row>
     <row r="555" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I555" s="7"/>
+      <c r="J555" s="8"/>
     </row>
     <row r="556" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I556" s="7"/>
+      <c r="J556" s="8"/>
     </row>
     <row r="557" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I557" s="7"/>
+      <c r="J557" s="8"/>
     </row>
     <row r="558" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I558" s="7"/>
+      <c r="J558" s="8"/>
     </row>
     <row r="559" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I559" s="7"/>
+      <c r="J559" s="8"/>
     </row>
     <row r="560" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I560" s="7"/>
+      <c r="J560" s="8"/>
     </row>
     <row r="561" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I561" s="7"/>
+      <c r="J561" s="8"/>
     </row>
     <row r="562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I562" s="7"/>
+      <c r="J562" s="8"/>
     </row>
     <row r="563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I563" s="7"/>
+      <c r="J563" s="8"/>
     </row>
     <row r="564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I564" s="7"/>
+      <c r="J564" s="8"/>
     </row>
     <row r="565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I565" s="7"/>
+      <c r="J565" s="8"/>
     </row>
     <row r="566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I566" s="7"/>
+      <c r="J566" s="8"/>
     </row>
     <row r="567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I567" s="7"/>
+      <c r="J567" s="8"/>
     </row>
     <row r="568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I568" s="7"/>
+      <c r="J568" s="8"/>
     </row>
     <row r="569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I569" s="7"/>
+      <c r="J569" s="8"/>
     </row>
     <row r="570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I570" s="7"/>
+      <c r="J570" s="8"/>
     </row>
     <row r="571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I571" s="7"/>
+      <c r="J571" s="8"/>
     </row>
     <row r="572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I572" s="7"/>
+      <c r="J572" s="8"/>
     </row>
     <row r="573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I573" s="7"/>
+      <c r="J573" s="8"/>
     </row>
     <row r="574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I574" s="7"/>
+      <c r="J574" s="8"/>
     </row>
     <row r="575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I575" s="7"/>
+      <c r="J575" s="8"/>
     </row>
     <row r="576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I576" s="7"/>
+      <c r="J576" s="8"/>
     </row>
     <row r="577" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I577" s="7"/>
+      <c r="J577" s="8"/>
     </row>
     <row r="578" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I578" s="7"/>
+      <c r="J578" s="8"/>
     </row>
     <row r="579" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I579" s="7"/>
+      <c r="J579" s="8"/>
     </row>
     <row r="580" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I580" s="7"/>
+      <c r="J580" s="8"/>
     </row>
     <row r="581" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I581" s="7"/>
+      <c r="J581" s="8"/>
     </row>
     <row r="582" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I582" s="7"/>
+      <c r="J582" s="8"/>
     </row>
     <row r="583" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I583" s="7"/>
+      <c r="J583" s="8"/>
     </row>
     <row r="584" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I584" s="7"/>
+      <c r="J584" s="8"/>
     </row>
     <row r="585" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I585" s="7"/>
+      <c r="J585" s="8"/>
     </row>
     <row r="586" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I586" s="7"/>
+      <c r="J586" s="8"/>
     </row>
     <row r="587" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I587" s="7"/>
+      <c r="J587" s="8"/>
     </row>
     <row r="588" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I588" s="7"/>
+      <c r="J588" s="8"/>
     </row>
     <row r="589" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I589" s="7"/>
+      <c r="J589" s="8"/>
     </row>
     <row r="590" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I590" s="7"/>
+      <c r="J590" s="8"/>
     </row>
     <row r="591" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I591" s="7"/>
+      <c r="J591" s="8"/>
     </row>
     <row r="592" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I592" s="7"/>
+      <c r="J592" s="8"/>
     </row>
     <row r="593" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I593" s="7"/>
+      <c r="J593" s="8"/>
     </row>
     <row r="594" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I594" s="7"/>
+      <c r="J594" s="8"/>
     </row>
     <row r="595" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I595" s="7"/>
+      <c r="J595" s="8"/>
     </row>
     <row r="596" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I596" s="7"/>
+      <c r="J596" s="8"/>
     </row>
     <row r="597" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I597" s="7"/>
+      <c r="J597" s="8"/>
     </row>
     <row r="598" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I598" s="7"/>
+      <c r="J598" s="8"/>
     </row>
     <row r="599" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I599" s="7"/>
+      <c r="J599" s="8"/>
     </row>
     <row r="600" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I600" s="7"/>
+      <c r="J600" s="8"/>
     </row>
     <row r="601" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I601" s="7"/>
+      <c r="J601" s="8"/>
     </row>
     <row r="602" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I602" s="7"/>
+      <c r="J602" s="8"/>
     </row>
     <row r="603" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I603" s="7"/>
+      <c r="J603" s="8"/>
     </row>
     <row r="604" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I604" s="7"/>
+      <c r="J604" s="8"/>
     </row>
     <row r="605" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I605" s="7"/>
+      <c r="J605" s="8"/>
     </row>
     <row r="606" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I606" s="7"/>
+      <c r="J606" s="8"/>
     </row>
     <row r="607" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I607" s="7"/>
+      <c r="J607" s="8"/>
     </row>
     <row r="608" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I608" s="7"/>
+      <c r="J608" s="8"/>
     </row>
     <row r="609" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I609" s="7"/>
+      <c r="J609" s="8"/>
     </row>
     <row r="610" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I610" s="7"/>
+      <c r="J610" s="8"/>
     </row>
     <row r="611" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I611" s="7"/>
+      <c r="J611" s="8"/>
     </row>
     <row r="612" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I612" s="7"/>
+      <c r="J612" s="8"/>
     </row>
     <row r="613" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I613" s="7"/>
+      <c r="J613" s="8"/>
     </row>
     <row r="614" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I614" s="7"/>
+      <c r="J614" s="8"/>
     </row>
     <row r="615" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I615" s="7"/>
+      <c r="J615" s="8"/>
     </row>
     <row r="616" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I616" s="7"/>
+      <c r="J616" s="8"/>
     </row>
     <row r="617" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I617" s="7"/>
+      <c r="J617" s="8"/>
     </row>
     <row r="618" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I618" s="7"/>
+      <c r="J618" s="8"/>
     </row>
     <row r="619" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I619" s="7"/>
+      <c r="J619" s="8"/>
     </row>
     <row r="620" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I620" s="7"/>
+      <c r="J620" s="8"/>
     </row>
     <row r="621" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I621" s="7"/>
+      <c r="J621" s="8"/>
     </row>
     <row r="622" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I622" s="7"/>
+      <c r="J622" s="8"/>
     </row>
     <row r="623" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I623" s="7"/>
+      <c r="J623" s="8"/>
     </row>
     <row r="624" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I624" s="7"/>
+      <c r="J624" s="8"/>
     </row>
     <row r="625" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I625" s="7"/>
+      <c r="J625" s="8"/>
     </row>
     <row r="626" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I626" s="7"/>
+      <c r="J626" s="8"/>
     </row>
     <row r="627" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I627" s="7"/>
+      <c r="J627" s="8"/>
     </row>
     <row r="628" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I628" s="7"/>
+      <c r="J628" s="8"/>
     </row>
     <row r="629" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I629" s="7"/>
+      <c r="J629" s="8"/>
     </row>
     <row r="630" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I630" s="7"/>
+      <c r="J630" s="8"/>
     </row>
     <row r="631" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I631" s="7"/>
+      <c r="J631" s="8"/>
     </row>
     <row r="632" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I632" s="7"/>
+      <c r="J632" s="8"/>
     </row>
     <row r="633" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I633" s="7"/>
+      <c r="J633" s="8"/>
     </row>
     <row r="634" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I634" s="7"/>
+      <c r="J634" s="8"/>
     </row>
     <row r="635" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I635" s="7"/>
+      <c r="J635" s="8"/>
     </row>
     <row r="636" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I636" s="7"/>
+      <c r="J636" s="8"/>
     </row>
     <row r="637" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I637" s="7"/>
+      <c r="J637" s="8"/>
     </row>
     <row r="638" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I638" s="7"/>
+      <c r="J638" s="8"/>
     </row>
     <row r="639" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I639" s="7"/>
+      <c r="J639" s="8"/>
     </row>
     <row r="640" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I640" s="7"/>
+      <c r="J640" s="8"/>
     </row>
     <row r="641" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I641" s="7"/>
+      <c r="J641" s="8"/>
     </row>
     <row r="642" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I642" s="7"/>
+      <c r="J642" s="8"/>
     </row>
     <row r="643" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I643" s="7"/>
+      <c r="J643" s="8"/>
     </row>
     <row r="644" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I644" s="7"/>
+      <c r="J644" s="8"/>
     </row>
     <row r="645" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I645" s="7"/>
+      <c r="J645" s="8"/>
     </row>
     <row r="646" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I646" s="7"/>
+      <c r="J646" s="8"/>
     </row>
     <row r="647" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I647" s="7"/>
+      <c r="J647" s="8"/>
     </row>
     <row r="648" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I648" s="7"/>
+      <c r="J648" s="8"/>
     </row>
     <row r="649" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I649" s="7"/>
+      <c r="J649" s="8"/>
     </row>
     <row r="650" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I650" s="7"/>
+      <c r="J650" s="8"/>
     </row>
     <row r="651" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I651" s="7"/>
+      <c r="J651" s="8"/>
     </row>
     <row r="652" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I652" s="7"/>
+      <c r="J652" s="8"/>
     </row>
     <row r="653" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I653" s="7"/>
+      <c r="J653" s="8"/>
     </row>
     <row r="654" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I654" s="7"/>
+      <c r="J654" s="8"/>
     </row>
     <row r="655" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I655" s="7"/>
+      <c r="J655" s="8"/>
     </row>
     <row r="656" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I656" s="7"/>
+      <c r="J656" s="8"/>
     </row>
     <row r="657" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I657" s="7"/>
+      <c r="J657" s="8"/>
     </row>
     <row r="658" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I658" s="7"/>
+      <c r="J658" s="8"/>
     </row>
     <row r="659" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I659" s="7"/>
+      <c r="J659" s="8"/>
     </row>
     <row r="660" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I660" s="7"/>
+      <c r="J660" s="8"/>
     </row>
     <row r="661" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I661" s="7"/>
+      <c r="J661" s="8"/>
     </row>
     <row r="662" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I662" s="7"/>
+      <c r="J662" s="8"/>
     </row>
     <row r="663" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I663" s="7"/>
+      <c r="J663" s="8"/>
     </row>
     <row r="664" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I664" s="7"/>
+      <c r="J664" s="8"/>
     </row>
     <row r="665" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I665" s="7"/>
+      <c r="J665" s="8"/>
     </row>
     <row r="666" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I666" s="7"/>
+      <c r="J666" s="8"/>
     </row>
     <row r="667" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I667" s="7"/>
+      <c r="J667" s="8"/>
     </row>
     <row r="668" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I668" s="7"/>
+      <c r="J668" s="8"/>
     </row>
     <row r="669" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I669" s="7"/>
+      <c r="J669" s="8"/>
     </row>
     <row r="670" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I670" s="7"/>
+      <c r="J670" s="8"/>
     </row>
     <row r="671" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I671" s="7"/>
+      <c r="J671" s="8"/>
     </row>
     <row r="672" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I672" s="7"/>
+      <c r="J672" s="8"/>
     </row>
     <row r="673" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I673" s="7"/>
+      <c r="J673" s="8"/>
     </row>
     <row r="674" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I674" s="7"/>
+      <c r="J674" s="8"/>
     </row>
     <row r="675" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I675" s="7"/>
+      <c r="J675" s="8"/>
     </row>
     <row r="676" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I676" s="7"/>
+      <c r="J676" s="8"/>
     </row>
     <row r="677" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I677" s="7"/>
+      <c r="J677" s="8"/>
     </row>
     <row r="678" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I678" s="7"/>
+      <c r="J678" s="8"/>
     </row>
     <row r="679" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I679" s="7"/>
+      <c r="J679" s="8"/>
     </row>
     <row r="680" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I680" s="7"/>
+      <c r="J680" s="8"/>
     </row>
     <row r="681" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I681" s="7"/>
+      <c r="J681" s="8"/>
     </row>
     <row r="682" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I682" s="7"/>
+      <c r="J682" s="8"/>
     </row>
     <row r="683" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I683" s="7"/>
+      <c r="J683" s="8"/>
     </row>
     <row r="684" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I684" s="7"/>
+      <c r="J684" s="8"/>
     </row>
     <row r="685" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I685" s="7"/>
+      <c r="J685" s="8"/>
     </row>
     <row r="686" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I686" s="7"/>
+      <c r="J686" s="8"/>
     </row>
     <row r="687" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I687" s="7"/>
+      <c r="J687" s="8"/>
     </row>
     <row r="688" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I688" s="7"/>
+      <c r="J688" s="8"/>
     </row>
     <row r="689" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I689" s="7"/>
+      <c r="J689" s="8"/>
     </row>
     <row r="690" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I690" s="7"/>
+      <c r="J690" s="8"/>
     </row>
     <row r="691" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I691" s="7"/>
+      <c r="J691" s="8"/>
     </row>
     <row r="692" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I692" s="7"/>
+      <c r="J692" s="8"/>
     </row>
     <row r="693" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I693" s="7"/>
+      <c r="J693" s="8"/>
     </row>
     <row r="694" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I694" s="7"/>
+      <c r="J694" s="8"/>
     </row>
     <row r="695" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I695" s="7"/>
+      <c r="J695" s="8"/>
     </row>
     <row r="696" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I696" s="7"/>
+      <c r="J696" s="8"/>
     </row>
     <row r="697" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I697" s="7"/>
+      <c r="J697" s="8"/>
     </row>
     <row r="698" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I698" s="7"/>
+      <c r="J698" s="8"/>
     </row>
     <row r="699" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I699" s="7"/>
+      <c r="J699" s="8"/>
     </row>
     <row r="700" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I700" s="7"/>
+      <c r="J700" s="8"/>
     </row>
     <row r="701" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I701" s="7"/>
+      <c r="J701" s="8"/>
     </row>
     <row r="702" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I702" s="7"/>
+      <c r="J702" s="8"/>
     </row>
     <row r="703" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I703" s="7"/>
+      <c r="J703" s="8"/>
     </row>
     <row r="704" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I704" s="7"/>
+      <c r="J704" s="8"/>
     </row>
     <row r="705" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I705" s="7"/>
+      <c r="J705" s="8"/>
     </row>
     <row r="706" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I706" s="7"/>
+      <c r="J706" s="8"/>
     </row>
     <row r="707" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I707" s="7"/>
+      <c r="J707" s="8"/>
     </row>
     <row r="708" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I708" s="7"/>
+      <c r="J708" s="8"/>
     </row>
     <row r="709" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I709" s="7"/>
+      <c r="J709" s="8"/>
     </row>
     <row r="710" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I710" s="7"/>
+      <c r="J710" s="8"/>
     </row>
     <row r="711" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I711" s="7"/>
+      <c r="J711" s="8"/>
     </row>
     <row r="712" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I712" s="7"/>
+      <c r="J712" s="8"/>
     </row>
     <row r="713" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I713" s="7"/>
+      <c r="J713" s="8"/>
     </row>
     <row r="714" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I714" s="7"/>
+      <c r="J714" s="8"/>
     </row>
     <row r="715" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I715" s="7"/>
+      <c r="J715" s="8"/>
     </row>
     <row r="716" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I716" s="7"/>
+      <c r="J716" s="8"/>
     </row>
     <row r="717" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I717" s="7"/>
+      <c r="J717" s="8"/>
     </row>
     <row r="718" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I718" s="7"/>
+      <c r="J718" s="8"/>
     </row>
     <row r="719" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I719" s="7"/>
+      <c r="J719" s="8"/>
     </row>
     <row r="720" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I720" s="7"/>
+      <c r="J720" s="8"/>
     </row>
     <row r="721" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I721" s="7"/>
+      <c r="J721" s="8"/>
     </row>
     <row r="722" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I722" s="7"/>
+      <c r="J722" s="8"/>
     </row>
     <row r="723" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I723" s="7"/>
+      <c r="J723" s="8"/>
     </row>
     <row r="724" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I724" s="7"/>
+      <c r="J724" s="8"/>
     </row>
     <row r="725" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I725" s="7"/>
+      <c r="J725" s="8"/>
     </row>
     <row r="726" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I726" s="7"/>
+      <c r="J726" s="8"/>
     </row>
     <row r="727" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I727" s="7"/>
+      <c r="J727" s="8"/>
     </row>
     <row r="728" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I728" s="7"/>
+      <c r="J728" s="8"/>
     </row>
     <row r="729" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I729" s="7"/>
+      <c r="J729" s="8"/>
     </row>
     <row r="730" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I730" s="7"/>
+      <c r="J730" s="8"/>
     </row>
     <row r="731" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I731" s="7"/>
+      <c r="J731" s="8"/>
     </row>
     <row r="732" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I732" s="7"/>
+      <c r="J732" s="8"/>
     </row>
     <row r="733" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I733" s="7"/>
+      <c r="J733" s="8"/>
     </row>
     <row r="734" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I734" s="7"/>
+      <c r="J734" s="8"/>
     </row>
     <row r="735" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I735" s="7"/>
+      <c r="J735" s="8"/>
     </row>
     <row r="736" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I736" s="7"/>
+      <c r="J736" s="8"/>
     </row>
     <row r="737" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I737" s="7"/>
+      <c r="J737" s="8"/>
     </row>
     <row r="738" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I738" s="7"/>
+      <c r="J738" s="8"/>
     </row>
     <row r="739" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I739" s="7"/>
+      <c r="J739" s="8"/>
     </row>
     <row r="740" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I740" s="7"/>
+      <c r="J740" s="8"/>
     </row>
     <row r="741" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I741" s="7"/>
+      <c r="J741" s="8"/>
     </row>
     <row r="742" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I742" s="7"/>
+      <c r="J742" s="8"/>
     </row>
     <row r="743" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I743" s="7"/>
+      <c r="J743" s="8"/>
     </row>
     <row r="744" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I744" s="7"/>
+      <c r="J744" s="8"/>
     </row>
     <row r="745" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I745" s="7"/>
+      <c r="J745" s="8"/>
     </row>
     <row r="746" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I746" s="7"/>
+      <c r="J746" s="8"/>
     </row>
     <row r="747" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I747" s="7"/>
+      <c r="J747" s="8"/>
     </row>
     <row r="748" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I748" s="7"/>
+      <c r="J748" s="8"/>
     </row>
     <row r="749" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I749" s="7"/>
+      <c r="J749" s="8"/>
     </row>
     <row r="750" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I750" s="7"/>
+      <c r="J750" s="8"/>
     </row>
     <row r="751" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I751" s="7"/>
+      <c r="J751" s="8"/>
     </row>
     <row r="752" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I752" s="7"/>
+      <c r="J752" s="8"/>
     </row>
     <row r="753" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I753" s="7"/>
+      <c r="J753" s="8"/>
     </row>
     <row r="754" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I754" s="7"/>
+      <c r="J754" s="8"/>
     </row>
     <row r="755" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I755" s="7"/>
+      <c r="J755" s="8"/>
     </row>
     <row r="756" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I756" s="7"/>
+      <c r="J756" s="8"/>
     </row>
     <row r="757" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I757" s="7"/>
+      <c r="J757" s="8"/>
     </row>
     <row r="758" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I758" s="7"/>
+      <c r="J758" s="8"/>
     </row>
     <row r="759" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I759" s="7"/>
+      <c r="J759" s="8"/>
     </row>
     <row r="760" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I760" s="7"/>
+      <c r="J760" s="8"/>
     </row>
     <row r="761" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I761" s="7"/>
+      <c r="J761" s="8"/>
     </row>
     <row r="762" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I762" s="7"/>
+      <c r="J762" s="8"/>
     </row>
     <row r="763" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I763" s="7"/>
+      <c r="J763" s="8"/>
     </row>
     <row r="764" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I764" s="7"/>
+      <c r="J764" s="8"/>
     </row>
     <row r="765" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I765" s="7"/>
+      <c r="J765" s="8"/>
     </row>
     <row r="766" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I766" s="7"/>
+      <c r="J766" s="8"/>
     </row>
     <row r="767" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I767" s="7"/>
+      <c r="J767" s="8"/>
     </row>
     <row r="768" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I768" s="7"/>
+      <c r="J768" s="8"/>
     </row>
     <row r="769" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I769" s="7"/>
+      <c r="J769" s="8"/>
     </row>
     <row r="770" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I770" s="7"/>
+      <c r="J770" s="8"/>
     </row>
     <row r="771" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I771" s="7"/>
+      <c r="J771" s="8"/>
     </row>
     <row r="772" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I772" s="7"/>
+      <c r="J772" s="8"/>
     </row>
     <row r="773" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I773" s="7"/>
+      <c r="J773" s="8"/>
     </row>
     <row r="774" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I774" s="7"/>
+      <c r="J774" s="8"/>
     </row>
     <row r="775" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I775" s="7"/>
+      <c r="J775" s="8"/>
     </row>
     <row r="776" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I776" s="7"/>
+      <c r="J776" s="8"/>
     </row>
     <row r="777" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I777" s="7"/>
+      <c r="J777" s="8"/>
     </row>
     <row r="778" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I778" s="7"/>
+      <c r="J778" s="8"/>
     </row>
     <row r="779" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I779" s="7"/>
+      <c r="J779" s="8"/>
     </row>
     <row r="780" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I780" s="7"/>
+      <c r="J780" s="8"/>
     </row>
     <row r="781" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I781" s="7"/>
+      <c r="J781" s="8"/>
     </row>
     <row r="782" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I782" s="7"/>
+      <c r="J782" s="8"/>
     </row>
     <row r="783" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I783" s="7"/>
+      <c r="J783" s="8"/>
     </row>
     <row r="784" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I784" s="7"/>
+      <c r="J784" s="8"/>
     </row>
     <row r="785" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I785" s="7"/>
+      <c r="J785" s="8"/>
     </row>
     <row r="786" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I786" s="7"/>
+      <c r="J786" s="8"/>
     </row>
     <row r="787" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I787" s="7"/>
+      <c r="J787" s="8"/>
     </row>
     <row r="788" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I788" s="7"/>
+      <c r="J788" s="8"/>
     </row>
     <row r="789" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I789" s="7"/>
+      <c r="J789" s="8"/>
     </row>
     <row r="790" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I790" s="7"/>
+      <c r="J790" s="8"/>
     </row>
     <row r="791" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I791" s="7"/>
+      <c r="J791" s="8"/>
     </row>
     <row r="792" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I792" s="7"/>
+      <c r="J792" s="8"/>
     </row>
     <row r="793" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I793" s="7"/>
+      <c r="J793" s="8"/>
     </row>
     <row r="794" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I794" s="7"/>
+      <c r="J794" s="8"/>
     </row>
     <row r="795" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I795" s="7"/>
+      <c r="J795" s="8"/>
     </row>
     <row r="796" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I796" s="7"/>
+      <c r="J796" s="8"/>
     </row>
     <row r="797" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I797" s="7"/>
+      <c r="J797" s="8"/>
     </row>
     <row r="798" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I798" s="7"/>
+      <c r="J798" s="8"/>
     </row>
     <row r="799" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I799" s="7"/>
+      <c r="J799" s="8"/>
     </row>
     <row r="800" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I800" s="7"/>
+      <c r="J800" s="8"/>
     </row>
     <row r="801" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I801" s="7"/>
+      <c r="J801" s="8"/>
     </row>
     <row r="802" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I802" s="7"/>
+      <c r="J802" s="8"/>
     </row>
     <row r="803" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I803" s="7"/>
+      <c r="J803" s="8"/>
     </row>
     <row r="804" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I804" s="7"/>
+      <c r="J804" s="8"/>
     </row>
     <row r="805" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I805" s="7"/>
+      <c r="J805" s="8"/>
     </row>
     <row r="806" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I806" s="7"/>
+      <c r="J806" s="8"/>
     </row>
     <row r="807" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I807" s="7"/>
+      <c r="J807" s="8"/>
     </row>
     <row r="808" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I808" s="7"/>
+      <c r="J808" s="8"/>
     </row>
     <row r="809" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I809" s="7"/>
+      <c r="J809" s="8"/>
     </row>
     <row r="810" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I810" s="7"/>
+      <c r="J810" s="8"/>
     </row>
     <row r="811" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I811" s="7"/>
+      <c r="J811" s="8"/>
     </row>
     <row r="812" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I812" s="7"/>
+      <c r="J812" s="8"/>
     </row>
     <row r="813" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I813" s="7"/>
+      <c r="J813" s="8"/>
     </row>
     <row r="814" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I814" s="7"/>
+      <c r="J814" s="8"/>
     </row>
     <row r="815" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I815" s="7"/>
+      <c r="J815" s="8"/>
     </row>
     <row r="816" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I816" s="7"/>
+      <c r="J816" s="8"/>
     </row>
     <row r="817" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I817" s="7"/>
+      <c r="J817" s="8"/>
     </row>
     <row r="818" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I818" s="7"/>
+      <c r="J818" s="8"/>
     </row>
     <row r="819" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I819" s="7"/>
+      <c r="J819" s="8"/>
     </row>
     <row r="820" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I820" s="7"/>
+      <c r="J820" s="8"/>
     </row>
     <row r="821" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I821" s="7"/>
+      <c r="J821" s="8"/>
     </row>
     <row r="822" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I822" s="7"/>
+      <c r="J822" s="8"/>
     </row>
     <row r="823" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I823" s="7"/>
+      <c r="J823" s="8"/>
     </row>
     <row r="824" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I824" s="7"/>
+      <c r="J824" s="8"/>
     </row>
     <row r="825" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I825" s="7"/>
+      <c r="J825" s="8"/>
     </row>
     <row r="826" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I826" s="7"/>
+      <c r="J826" s="8"/>
     </row>
     <row r="827" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I827" s="7"/>
+      <c r="J827" s="8"/>
     </row>
     <row r="828" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I828" s="7"/>
+      <c r="J828" s="8"/>
     </row>
     <row r="829" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I829" s="7"/>
+      <c r="J829" s="8"/>
     </row>
     <row r="830" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I830" s="7"/>
+      <c r="J830" s="8"/>
     </row>
     <row r="831" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I831" s="7"/>
+      <c r="J831" s="8"/>
     </row>
     <row r="832" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I832" s="7"/>
+      <c r="J832" s="8"/>
     </row>
     <row r="833" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I833" s="7"/>
+      <c r="J833" s="8"/>
     </row>
     <row r="834" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I834" s="7"/>
+      <c r="J834" s="8"/>
     </row>
     <row r="835" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I835" s="7"/>
+      <c r="J835" s="8"/>
     </row>
     <row r="836" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I836" s="7"/>
+      <c r="J836" s="8"/>
     </row>
     <row r="837" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I837" s="7"/>
+      <c r="J837" s="8"/>
     </row>
     <row r="838" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I838" s="7"/>
+      <c r="J838" s="8"/>
     </row>
     <row r="839" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I839" s="7"/>
+      <c r="J839" s="8"/>
     </row>
     <row r="840" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I840" s="7"/>
+      <c r="J840" s="8"/>
     </row>
     <row r="841" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I841" s="7"/>
+      <c r="J841" s="8"/>
     </row>
     <row r="842" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I842" s="7"/>
+      <c r="J842" s="8"/>
     </row>
     <row r="843" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I843" s="7"/>
+      <c r="J843" s="8"/>
     </row>
     <row r="844" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I844" s="7"/>
+      <c r="J844" s="8"/>
     </row>
     <row r="845" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I845" s="7"/>
+      <c r="J845" s="8"/>
     </row>
     <row r="846" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I846" s="7"/>
+      <c r="J846" s="8"/>
     </row>
     <row r="847" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I847" s="7"/>
+      <c r="J847" s="8"/>
     </row>
     <row r="848" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I848" s="7"/>
+      <c r="J848" s="8"/>
     </row>
     <row r="849" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I849" s="7"/>
+      <c r="J849" s="8"/>
     </row>
     <row r="850" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I850" s="7"/>
+      <c r="J850" s="8"/>
     </row>
     <row r="851" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I851" s="7"/>
+      <c r="J851" s="8"/>
     </row>
     <row r="852" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I852" s="7"/>
+      <c r="J852" s="8"/>
     </row>
     <row r="853" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I853" s="7"/>
+      <c r="J853" s="8"/>
     </row>
     <row r="854" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I854" s="7"/>
+      <c r="J854" s="8"/>
     </row>
     <row r="855" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I855" s="7"/>
+      <c r="J855" s="8"/>
     </row>
     <row r="856" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I856" s="7"/>
+      <c r="J856" s="8"/>
     </row>
     <row r="857" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I857" s="7"/>
+      <c r="J857" s="8"/>
     </row>
     <row r="858" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I858" s="7"/>
+      <c r="J858" s="8"/>
     </row>
     <row r="859" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I859" s="7"/>
+      <c r="J859" s="8"/>
     </row>
     <row r="860" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I860" s="7"/>
+      <c r="J860" s="8"/>
     </row>
     <row r="861" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I861" s="7"/>
+      <c r="J861" s="8"/>
     </row>
     <row r="862" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I862" s="7"/>
+      <c r="J862" s="8"/>
     </row>
     <row r="863" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I863" s="7"/>
+      <c r="J863" s="8"/>
     </row>
     <row r="864" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I864" s="7"/>
+      <c r="J864" s="8"/>
     </row>
     <row r="865" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I865" s="7"/>
+      <c r="J865" s="8"/>
     </row>
     <row r="866" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I866" s="7"/>
+      <c r="J866" s="8"/>
     </row>
     <row r="867" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I867" s="7"/>
+      <c r="J867" s="8"/>
     </row>
     <row r="868" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I868" s="7"/>
+      <c r="J868" s="8"/>
     </row>
     <row r="869" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I869" s="7"/>
+      <c r="J869" s="8"/>
     </row>
     <row r="870" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I870" s="7"/>
+      <c r="J870" s="8"/>
     </row>
     <row r="871" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I871" s="7"/>
+      <c r="J871" s="8"/>
     </row>
     <row r="872" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I872" s="7"/>
+      <c r="J872" s="8"/>
     </row>
     <row r="873" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I873" s="7"/>
+      <c r="J873" s="8"/>
     </row>
     <row r="874" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I874" s="7"/>
+      <c r="J874" s="8"/>
     </row>
     <row r="875" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I875" s="7"/>
+      <c r="J875" s="8"/>
     </row>
     <row r="876" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I876" s="7"/>
+      <c r="J876" s="8"/>
     </row>
     <row r="877" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I877" s="7"/>
+      <c r="J877" s="8"/>
     </row>
     <row r="878" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I878" s="7"/>
+      <c r="J878" s="8"/>
     </row>
     <row r="879" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I879" s="7"/>
+      <c r="J879" s="8"/>
     </row>
     <row r="880" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I880" s="7"/>
+      <c r="J880" s="8"/>
     </row>
     <row r="881" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I881" s="7"/>
+      <c r="J881" s="8"/>
     </row>
     <row r="882" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I882" s="7"/>
+      <c r="J882" s="8"/>
     </row>
     <row r="883" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I883" s="7"/>
+      <c r="J883" s="8"/>
     </row>
     <row r="884" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I884" s="7"/>
+      <c r="J884" s="8"/>
     </row>
     <row r="885" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I885" s="7"/>
+      <c r="J885" s="8"/>
     </row>
     <row r="886" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I886" s="7"/>
+      <c r="J886" s="8"/>
     </row>
     <row r="887" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I887" s="7"/>
+      <c r="J887" s="8"/>
     </row>
     <row r="888" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I888" s="7"/>
+      <c r="J888" s="8"/>
     </row>
     <row r="889" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I889" s="7"/>
+      <c r="J889" s="8"/>
     </row>
     <row r="890" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I890" s="7"/>
+      <c r="J890" s="8"/>
     </row>
     <row r="891" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I891" s="7"/>
+      <c r="J891" s="8"/>
     </row>
     <row r="892" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I892" s="7"/>
+      <c r="J892" s="8"/>
     </row>
     <row r="893" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I893" s="7"/>
+      <c r="J893" s="8"/>
     </row>
     <row r="894" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I894" s="7"/>
+      <c r="J894" s="8"/>
     </row>
     <row r="895" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I895" s="7"/>
+      <c r="J895" s="8"/>
     </row>
     <row r="896" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I896" s="7"/>
+      <c r="J896" s="8"/>
     </row>
     <row r="897" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I897" s="7"/>
+      <c r="J897" s="8"/>
     </row>
     <row r="898" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I898" s="7"/>
+      <c r="J898" s="8"/>
     </row>
     <row r="899" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I899" s="7"/>
+      <c r="J899" s="8"/>
     </row>
     <row r="900" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I900" s="7"/>
+      <c r="J900" s="8"/>
     </row>
     <row r="901" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I901" s="7"/>
+      <c r="J901" s="8"/>
     </row>
     <row r="902" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I902" s="7"/>
+      <c r="J902" s="8"/>
     </row>
     <row r="903" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I903" s="7"/>
+      <c r="J903" s="8"/>
     </row>
     <row r="904" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I904" s="7"/>
+      <c r="J904" s="8"/>
     </row>
     <row r="905" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I905" s="7"/>
+      <c r="J905" s="8"/>
     </row>
     <row r="906" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I906" s="7"/>
+      <c r="J906" s="8"/>
     </row>
     <row r="907" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I907" s="7"/>
+      <c r="J907" s="8"/>
     </row>
     <row r="908" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I908" s="7"/>
+      <c r="J908" s="8"/>
     </row>
     <row r="909" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I909" s="7"/>
+      <c r="J909" s="8"/>
     </row>
     <row r="910" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I910" s="7"/>
+      <c r="J910" s="8"/>
     </row>
     <row r="911" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I911" s="7"/>
+      <c r="J911" s="8"/>
     </row>
     <row r="912" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I912" s="7"/>
+      <c r="J912" s="8"/>
     </row>
     <row r="913" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I913" s="7"/>
+      <c r="J913" s="8"/>
     </row>
     <row r="914" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I914" s="7"/>
+      <c r="J914" s="8"/>
     </row>
     <row r="915" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I915" s="7"/>
+      <c r="J915" s="8"/>
     </row>
     <row r="916" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I916" s="7"/>
+      <c r="J916" s="8"/>
     </row>
     <row r="917" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I917" s="7"/>
+      <c r="J917" s="8"/>
     </row>
     <row r="918" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I918" s="7"/>
+      <c r="J918" s="8"/>
     </row>
     <row r="919" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I919" s="7"/>
+      <c r="J919" s="8"/>
     </row>
     <row r="920" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I920" s="7"/>
+      <c r="J920" s="8"/>
     </row>
     <row r="921" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I921" s="7"/>
+      <c r="J921" s="8"/>
     </row>
     <row r="922" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I922" s="7"/>
+      <c r="J922" s="8"/>
     </row>
     <row r="923" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I923" s="7"/>
+      <c r="J923" s="8"/>
     </row>
     <row r="924" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I924" s="7"/>
+      <c r="J924" s="8"/>
     </row>
     <row r="925" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I925" s="7"/>
+      <c r="J925" s="8"/>
     </row>
     <row r="926" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I926" s="7"/>
+      <c r="J926" s="8"/>
     </row>
     <row r="927" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I927" s="7"/>
+      <c r="J927" s="8"/>
     </row>
     <row r="928" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I928" s="7"/>
+      <c r="J928" s="8"/>
     </row>
     <row r="929" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I929" s="7"/>
+      <c r="J929" s="8"/>
     </row>
     <row r="930" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I930" s="7"/>
+      <c r="J930" s="8"/>
     </row>
     <row r="931" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I931" s="7"/>
+      <c r="J931" s="8"/>
     </row>
     <row r="932" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I932" s="7"/>
+      <c r="J932" s="8"/>
     </row>
     <row r="933" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I933" s="7"/>
+      <c r="J933" s="8"/>
     </row>
     <row r="934" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I934" s="7"/>
+      <c r="J934" s="8"/>
     </row>
     <row r="935" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I935" s="7"/>
+      <c r="J935" s="8"/>
     </row>
     <row r="936" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I936" s="7"/>
+      <c r="J936" s="8"/>
     </row>
     <row r="937" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I937" s="7"/>
+      <c r="J937" s="8"/>
     </row>
     <row r="938" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I938" s="7"/>
+      <c r="J938" s="8"/>
     </row>
     <row r="939" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I939" s="7"/>
+      <c r="J939" s="8"/>
     </row>
     <row r="940" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I940" s="7"/>
+      <c r="J940" s="8"/>
     </row>
     <row r="941" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I941" s="7"/>
+      <c r="J941" s="8"/>
     </row>
     <row r="942" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I942" s="7"/>
+      <c r="J942" s="8"/>
     </row>
     <row r="943" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I943" s="7"/>
+      <c r="J943" s="8"/>
     </row>
     <row r="944" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I944" s="7"/>
+      <c r="J944" s="8"/>
     </row>
     <row r="945" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I945" s="7"/>
+      <c r="J945" s="8"/>
     </row>
     <row r="946" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I946" s="7"/>
+      <c r="J946" s="8"/>
     </row>
     <row r="947" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I947" s="7"/>
+      <c r="J947" s="8"/>
     </row>
     <row r="948" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I948" s="7"/>
+      <c r="J948" s="8"/>
     </row>
     <row r="949" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I949" s="7"/>
+      <c r="J949" s="8"/>
     </row>
     <row r="950" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I950" s="7"/>
+      <c r="J950" s="8"/>
     </row>
     <row r="951" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I951" s="7"/>
+      <c r="J951" s="8"/>
     </row>
     <row r="952" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I952" s="7"/>
+      <c r="J952" s="8"/>
     </row>
     <row r="953" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I953" s="7"/>
+      <c r="J953" s="8"/>
     </row>
     <row r="954" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I954" s="7"/>
+      <c r="J954" s="8"/>
     </row>
     <row r="955" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I955" s="7"/>
+      <c r="J955" s="8"/>
     </row>
     <row r="956" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I956" s="7"/>
+      <c r="J956" s="8"/>
     </row>
     <row r="957" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I957" s="7"/>
+      <c r="J957" s="8"/>
     </row>
     <row r="958" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I958" s="7"/>
+      <c r="J958" s="8"/>
     </row>
     <row r="959" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I959" s="7"/>
+      <c r="J959" s="8"/>
     </row>
     <row r="960" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I960" s="7"/>
+      <c r="J960" s="8"/>
     </row>
     <row r="961" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I961" s="7"/>
+      <c r="J961" s="8"/>
     </row>
     <row r="962" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I962" s="7"/>
+      <c r="J962" s="8"/>
     </row>
     <row r="963" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I963" s="7"/>
+      <c r="J963" s="8"/>
     </row>
     <row r="964" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I964" s="7"/>
+      <c r="J964" s="8"/>
     </row>
     <row r="965" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I965" s="7"/>
+      <c r="J965" s="8"/>
     </row>
     <row r="966" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I966" s="7"/>
+      <c r="J966" s="8"/>
     </row>
     <row r="967" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I967" s="7"/>
+      <c r="J967" s="8"/>
     </row>
     <row r="968" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I968" s="7"/>
+      <c r="J968" s="8"/>
     </row>
     <row r="969" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I969" s="7"/>
+      <c r="J969" s="8"/>
     </row>
     <row r="970" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I970" s="7"/>
+      <c r="J970" s="8"/>
     </row>
     <row r="971" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I971" s="7"/>
+      <c r="J971" s="8"/>
     </row>
     <row r="972" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I972" s="7"/>
+      <c r="J972" s="8"/>
     </row>
     <row r="973" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I973" s="7"/>
+      <c r="J973" s="8"/>
     </row>
     <row r="974" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I974" s="7"/>
+      <c r="J974" s="8"/>
     </row>
     <row r="975" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I975" s="7"/>
+      <c r="J975" s="8"/>
     </row>
     <row r="976" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I976" s="7"/>
+      <c r="J976" s="8"/>
     </row>
     <row r="977" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I977" s="7"/>
+      <c r="J977" s="8"/>
     </row>
     <row r="978" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I978" s="7"/>
+      <c r="J978" s="8"/>
     </row>
     <row r="979" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I979" s="7"/>
+      <c r="J979" s="8"/>
     </row>
     <row r="980" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I980" s="7"/>
+      <c r="J980" s="8"/>
     </row>
     <row r="981" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I981" s="7"/>
+      <c r="J981" s="8"/>
     </row>
     <row r="982" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I982" s="7"/>
+      <c r="J982" s="8"/>
     </row>
     <row r="983" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I983" s="7"/>
+      <c r="J983" s="8"/>
     </row>
     <row r="984" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I984" s="7"/>
+      <c r="J984" s="8"/>
     </row>
     <row r="985" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I985" s="7"/>
+      <c r="J985" s="8"/>
     </row>
     <row r="986" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I986" s="7"/>
+      <c r="J986" s="8"/>
     </row>
     <row r="987" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I987" s="7"/>
+      <c r="J987" s="8"/>
     </row>
     <row r="988" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I988" s="7"/>
+      <c r="J988" s="8"/>
     </row>
     <row r="989" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I989" s="7"/>
+      <c r="J989" s="8"/>
     </row>
     <row r="990" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I990" s="7"/>
+      <c r="J990" s="8"/>
     </row>
     <row r="991" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I991" s="7"/>
+      <c r="J991" s="8"/>
     </row>
     <row r="992" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I992" s="7"/>
+      <c r="J992" s="8"/>
     </row>
     <row r="993" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I993" s="7"/>
+      <c r="J993" s="8"/>
     </row>
     <row r="994" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I994" s="7"/>
+      <c r="J994" s="8"/>
     </row>
     <row r="995" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I995" s="7"/>
+      <c r="J995" s="8"/>
     </row>
     <row r="996" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I996" s="7"/>
+      <c r="J996" s="8"/>
     </row>
     <row r="997" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I997" s="7"/>
+      <c r="J997" s="8"/>
     </row>
     <row r="998" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I998" s="7"/>
+      <c r="J998" s="8"/>
     </row>
     <row r="999" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I999" s="7"/>
+      <c r="J999" s="8"/>
     </row>
     <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I1000" s="7"/>
+      <c r="J1000" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I1000" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J1000" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>